<commit_message>
added new Data folder and inside this folder INPUT,OUTPUT/TEP filders are available
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dinuka Thilakarathne\OneDrive\Documents\UiPath\Re-Usable Edited Framwork\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC74D233-EED3-42E6-8643-B0930365A798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -160,18 +160,6 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
-  </si>
-  <si>
-    <t>D:\RE Projects\RE Test\</t>
-  </si>
-  <si>
-    <t>main_FilePath</t>
-  </si>
-  <si>
-    <t>screenshotFolderPath</t>
-  </si>
-  <si>
-    <t>C:\Users\Dinuka Thilakarathne\OneDrive\Documents\UiPath\Re-Usable Edited Framwork\Exceptions_Screenshots\</t>
   </si>
 </sst>
 </file>
@@ -224,10 +212,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -547,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z995"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -627,22 +615,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
-      </c>
-    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1631,6 +1605,9 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
+    <row r="996" ht="14.25" customHeight="1"/>
+    <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2805,7 +2782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
modified login sequence and added login extra validation exceptions and 3 times login attempts and error notification template
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dinuka Thilakarathne\OneDrive\Documents\UiPath\Re-Usable Edited Framwork\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A89251-B70B-4B3B-8BCF-4959DE21A352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +160,36 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>process url</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/60645613/oracle-stored-procedure-not-working-pls-00306</t>
+  </si>
+  <si>
+    <t>Main_FolderPath</t>
+  </si>
+  <si>
+    <t>C:\Users\Dinuka Thilakarathne\OneDrive\Documents\UiPath\Re-Usable Edited Framwork\Data\Output\</t>
+  </si>
+  <si>
+    <t>Output_FolderPath</t>
+  </si>
+  <si>
+    <t>Temp_FolderPath</t>
+  </si>
+  <si>
+    <t>ScreenShot_FolderPath</t>
+  </si>
+  <si>
+    <t>C:\Users\Dinuka Thilakarathne\OneDrive\Documents\UiPath\Re-Usable Edited Framwork\Data\Output\Temp\</t>
+  </si>
+  <si>
+    <t>C:\Users\Dinuka Thilakarathne\OneDrive\Documents\UiPath\Re-Usable Edited Framwork\Data\Output\ScreenShots\</t>
+  </si>
+  <si>
+    <t>C:\Users\Dinuka Thilakarathne\OneDrive\Documents\UiPath\Re-Usable Edited Framwork\Data\Output\Output Files\</t>
   </si>
 </sst>
 </file>
@@ -212,10 +242,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -537,14 +567,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="2" max="2" width="46.44140625" customWidth="1"/>
     <col min="3" max="3" width="81.44140625" customWidth="1"/>
     <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
@@ -615,11 +645,46 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1620,7 +1685,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A18" sqref="A18:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2782,7 +2847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
added new outlook email and created a new outlook email connection and testes it send email list read from config and text file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dinuka Thilakarathne\OneDrive\Documents\UiPath\Re-Usable Edited Framwork\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D872D8-B0A2-4F0D-A03C-7E079CA7D4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771EAE19-E7EA-40BE-A12C-0E326E4DA103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>Modern Folder</t>
+  </si>
+  <si>
+    <t>dthilakarathne@innobothealth.com,dthilakarathne@innobothealth.com</t>
   </si>
 </sst>
 </file>
@@ -587,14 +590,14 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="46.44140625" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="1" max="1" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="105" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -711,14 +714,14 @@
         <v>55</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>